<commit_message>
updated the landing page (actions.html, actions.css) to display slideshow while result is fetched, add close button to close window
</commit_message>
<xml_diff>
--- a/bugs/bugsTracking.xlsx
+++ b/bugs/bugsTracking.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
   <si>
     <t>#</t>
   </si>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t>Add tone analyzer to output</t>
+  </si>
+  <si>
+    <t>make 6 keywords result instead of 5 for better display</t>
   </si>
 </sst>
 </file>
@@ -514,10 +517,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B4"/>
+  <dimension ref="A2:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,6 +552,14 @@
         <v>17</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>